<commit_message>
Stun now cancels abilities
</commit_message>
<xml_diff>
--- a/Assets/Resources/Abilities.xlsx
+++ b/Assets/Resources/Abilities.xlsx
@@ -64,8 +64,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -93,9 +101,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -429,7 +438,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -475,7 +484,7 @@
         <v>5</v>
       </c>
       <c r="D2">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -498,7 +507,7 @@
         <v>2</v>
       </c>
       <c r="D3">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -538,13 +547,13 @@
         <v>8</v>
       </c>
       <c r="B5">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C5">
         <v>30</v>
       </c>
       <c r="D5">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="E5">
         <v>3</v>
@@ -566,8 +575,8 @@
       <c r="C6">
         <v>5</v>
       </c>
-      <c r="D6">
-        <v>50</v>
+      <c r="D6" s="2">
+        <v>5</v>
       </c>
       <c r="E6">
         <v>3</v>

</xml_diff>

<commit_message>
Only one skill at a time!
</commit_message>
<xml_diff>
--- a/Assets/Resources/Abilities.xlsx
+++ b/Assets/Resources/Abilities.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17280" windowHeight="6924"/>
   </bookViews>
   <sheets>
     <sheet name="Abilities" sheetId="1" r:id="rId1"/>
@@ -438,7 +438,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -484,13 +484,13 @@
         <v>5</v>
       </c>
       <c r="D2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G2">
         <v>0</v>
@@ -507,7 +507,7 @@
         <v>2</v>
       </c>
       <c r="D3">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -553,7 +553,7 @@
         <v>30</v>
       </c>
       <c r="D5">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E5">
         <v>3</v>
@@ -576,7 +576,7 @@
         <v>5</v>
       </c>
       <c r="D6" s="2">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="E6">
         <v>3</v>

</xml_diff>

<commit_message>
All abilities! Good excel importing!
</commit_message>
<xml_diff>
--- a/Assets/Resources/Abilities.xlsx
+++ b/Assets/Resources/Abilities.xlsx
@@ -8,8 +8,9 @@
   </bookViews>
   <sheets>
     <sheet name="Abilities" sheetId="1" r:id="rId1"/>
+    <sheet name="Characters" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="29">
   <si>
     <t>Heal</t>
   </si>
@@ -58,6 +59,54 @@
   </si>
   <si>
     <t>Swap</t>
+  </si>
+  <si>
+    <t>CharacterType</t>
+  </si>
+  <si>
+    <t>Boss</t>
+  </si>
+  <si>
+    <t>Barrier</t>
+  </si>
+  <si>
+    <t>Swapper</t>
+  </si>
+  <si>
+    <t>Healer</t>
+  </si>
+  <si>
+    <t>Nuker</t>
+  </si>
+  <si>
+    <t>Stuner</t>
+  </si>
+  <si>
+    <t>Poker</t>
+  </si>
+  <si>
+    <t>Health</t>
+  </si>
+  <si>
+    <t>StartStun</t>
+  </si>
+  <si>
+    <t>Ditto</t>
+  </si>
+  <si>
+    <t>Copy</t>
+  </si>
+  <si>
+    <t>Taunt</t>
+  </si>
+  <si>
+    <t>Taunter</t>
+  </si>
+  <si>
+    <t>Buffer</t>
+  </si>
+  <si>
+    <t>Buff</t>
   </si>
 </sst>
 </file>
@@ -133,6 +182,18 @@
     <tableColumn id="5" name="effectDuration"/>
     <tableColumn id="6" name="ticks"/>
     <tableColumn id="8" name="objectSpeed"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:C11" totalsRowShown="0">
+  <autoFilter ref="A1:C11"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="CharacterType"/>
+    <tableColumn id="2" name="Health"/>
+    <tableColumn id="9" name="StartStun"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -435,10 +496,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -593,7 +654,7 @@
         <v>12</v>
       </c>
       <c r="B7">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="C7">
         <v>5</v>
@@ -608,6 +669,75 @@
         <v>0</v>
       </c>
       <c r="G7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>10</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>10</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>3</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>5</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
+      <c r="E10">
+        <v>5</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
         <v>0</v>
       </c>
     </row>
@@ -618,4 +748,149 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="23.77734375" customWidth="1"/>
+    <col min="3" max="8" width="9.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2">
+        <f>SUM(B3:B11)</f>
+        <v>850</v>
+      </c>
+      <c r="C2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3">
+        <v>100</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4">
+        <v>100</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5">
+        <v>50</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6">
+        <v>100</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7">
+        <v>100</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8">
+        <v>100</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9">
+        <v>100</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10">
+        <v>100</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11">
+        <v>100</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>